<commit_message>
Update of the model to support Verifiable Presentations
</commit_message>
<xml_diff>
--- a/ECDI_model_individuals.xlsx
+++ b/ECDI_model_individuals.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\piete\Dropbox\workfolder\cogni\projects\ecdi\work\v0.3.0.draft\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\piete\Dropbox\workfolder\cogni\projects\ecdi\work\v0.4.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35B1E428-484C-4E9E-86BF-5DCAAD3C9FEC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C246EB57-22B5-4497-A59D-66A62791994E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{A43DAC4D-3848-4EAE-AC0D-3E6B152FBB9D}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" firstSheet="11" activeTab="15" xr2:uid="{A43DAC4D-3848-4EAE-AC0D-3E6B152FBB9D}"/>
   </bookViews>
   <sheets>
     <sheet name="Individuals" sheetId="8" r:id="rId1"/>
@@ -28,9 +28,11 @@
     <sheet name="AssessmentTypes" sheetId="4" r:id="rId13"/>
     <sheet name="MediaTypes" sheetId="10" r:id="rId14"/>
     <sheet name="ContentEncodingTypes" sheetId="11" r:id="rId15"/>
+    <sheet name="VerificationTypes" sheetId="29" r:id="rId16"/>
+    <sheet name="VerificationStatusses" sheetId="30" r:id="rId17"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId16"/>
+    <externalReference r:id="rId18"/>
   </externalReferences>
   <definedNames>
     <definedName name="_1__xlcn.WorksheetConnection_Core_Vocabularies_template.xlsxCoreVocabularies1" hidden="1">[1]!CoreVocabularies[#Data]</definedName>
@@ -108,7 +110,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="210">
   <si>
     <t>Class</t>
   </si>
@@ -681,6 +683,63 @@
   </si>
   <si>
     <t>ESCO skossified version</t>
+  </si>
+  <si>
+    <t>Europass Standard List of Verification Types.</t>
+  </si>
+  <si>
+    <t>Europass Standard List of Verification Statusses</t>
+  </si>
+  <si>
+    <t>http://data.europa.eu/europass/codeList/verificationTypes</t>
+  </si>
+  <si>
+    <t>Europass Standard List of Verification Types</t>
+  </si>
+  <si>
+    <t>http://data.europa.eu/europass/codeList/verificationStatusses</t>
+  </si>
+  <si>
+    <t>http://data.europa.eu/europass/verificationType/format</t>
+  </si>
+  <si>
+    <t>http://data.europa.eu/europass/verificationType/seal</t>
+  </si>
+  <si>
+    <t>http://data.europa.eu/europass/verificationType/owner</t>
+  </si>
+  <si>
+    <t>http://data.europa.eu/europass/verificationType/revocation</t>
+  </si>
+  <si>
+    <t>http://data.europa.eu/europass/verificationStatus/green</t>
+  </si>
+  <si>
+    <t>http://data.europa.eu/europass/verificationStatus/red</t>
+  </si>
+  <si>
+    <t>http://data.europa.eu/europass/verificationStatus/gray</t>
+  </si>
+  <si>
+    <t>green</t>
+  </si>
+  <si>
+    <t>red</t>
+  </si>
+  <si>
+    <t>gray</t>
+  </si>
+  <si>
+    <t>format</t>
+  </si>
+  <si>
+    <t>seal</t>
+  </si>
+  <si>
+    <t>owner</t>
+  </si>
+  <si>
+    <t>revocation</t>
   </si>
 </sst>
 </file>
@@ -1211,10 +1270,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D7C65FB-96B7-4669-B8D7-C5F8AC7942F1}">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:K38"/>
+  <dimension ref="A1:K40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33:A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1321,138 +1380,120 @@
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="12" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="12" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="12" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="12" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="12" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="12" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="12" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="12" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="12" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="12" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="12" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="12" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A30" s="12"/>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A31" s="11" t="s">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A30" s="12" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A31" s="12" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A32" s="12"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A33" s="11" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A32" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="B32" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="C32" s="12" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A33" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="B33" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="C33" s="12" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="12" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B34" s="12" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C34" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="D34" s="12" t="s">
-        <v>190</v>
+        <v>29</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="12" t="s">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="B35" s="12" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C35" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="D35" s="12" t="s">
-        <v>190</v>
+        <v>32</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="12" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B36" s="12" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C36" s="12" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="D36" s="12" t="s">
         <v>190</v>
@@ -1460,23 +1501,51 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="12" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B37" s="12" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C37" s="12" t="s">
-        <v>42</v>
+        <v>37</v>
+      </c>
+      <c r="D37" s="12" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="B38" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="C38" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="D38" s="12" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A39" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B39" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="C39" s="12" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A40" s="12" t="s">
         <v>185</v>
       </c>
-      <c r="B38" s="12" t="s">
+      <c r="B40" s="12" t="s">
         <v>186</v>
       </c>
-      <c r="C38" s="12" t="s">
+      <c r="C40" s="12" t="s">
         <v>187</v>
       </c>
     </row>
@@ -1860,7 +1929,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection sqref="A1:E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1976,7 +2045,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection sqref="A1:E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2096,7 +2165,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2182,6 +2251,233 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1" xr:uid="{A9C3A4FB-385F-4D61-A169-BACA2367239E}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95D8780A-898E-42B0-8AD8-52D762622FBE}">
+  <dimension ref="A1:E8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="20.26171875" customWidth="1"/>
+    <col min="2" max="2" width="48.83984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.15625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.89453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.68359375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" s="6"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="6"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="7"/>
+      <c r="B3" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="D3" s="7"/>
+      <c r="E3" s="4"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" s="6"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="6"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" t="s">
+        <v>196</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="E5" s="4"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B6" t="s">
+        <v>197</v>
+      </c>
+      <c r="C6" t="s">
+        <v>207</v>
+      </c>
+      <c r="D6" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B7" t="s">
+        <v>198</v>
+      </c>
+      <c r="C7" t="s">
+        <v>208</v>
+      </c>
+      <c r="D7" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B8" t="s">
+        <v>199</v>
+      </c>
+      <c r="C8" t="s">
+        <v>209</v>
+      </c>
+      <c r="D8" t="s">
+        <v>209</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{23B72603-5D70-4560-A169-4FE75E51A07B}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75A3CBA9-3D92-4142-B742-C4820FE9080E}">
+  <dimension ref="A1:E7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="18.68359375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="50.41796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.9453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.89453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.68359375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" s="6"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="6"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="7"/>
+      <c r="B3" t="s">
+        <v>195</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="D3" s="7"/>
+      <c r="E3" s="4"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" s="6"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="6"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="E5" s="4"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B6" t="s">
+        <v>201</v>
+      </c>
+      <c r="C6" t="s">
+        <v>204</v>
+      </c>
+      <c r="D6" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B7" t="s">
+        <v>202</v>
+      </c>
+      <c r="C7" t="s">
+        <v>205</v>
+      </c>
+      <c r="D7" t="s">
+        <v>205</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{D7BF9801-1BBA-418B-842F-3D17F63ECAAB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3217,18 +3513,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3251,14 +3547,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{67DC0167-6166-49C1-807E-C2398B5CAF50}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E2C7F53A-8E89-4CCC-9F6C-1071910C1BD9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
@@ -3273,4 +3561,12 @@
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{67DC0167-6166-49C1-807E-C2398B5CAF50}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Major update to xsd 0.4.0 based on data model 0.5.0
</commit_message>
<xml_diff>
--- a/ECDI_model_individuals.xlsx
+++ b/ECDI_model_individuals.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\piete\Dropbox\workfolder\cogni\projects\ecdi\work\v0.4.0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\antho\Repositories\EDCI-Data-Model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C246EB57-22B5-4497-A59D-66A62791994E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65FE9EC6-B067-4047-A133-9FCA50975BA2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" firstSheet="11" activeTab="15" xr2:uid="{A43DAC4D-3848-4EAE-AC0D-3E6B152FBB9D}"/>
+    <workbookView xWindow="-10500" yWindow="-21720" windowWidth="51840" windowHeight="21840" firstSheet="8" activeTab="19" xr2:uid="{A43DAC4D-3848-4EAE-AC0D-3E6B152FBB9D}"/>
   </bookViews>
   <sheets>
     <sheet name="Individuals" sheetId="8" r:id="rId1"/>
@@ -30,49 +30,72 @@
     <sheet name="ContentEncodingTypes" sheetId="11" r:id="rId15"/>
     <sheet name="VerificationTypes" sheetId="29" r:id="rId16"/>
     <sheet name="VerificationStatusses" sheetId="30" r:id="rId17"/>
+    <sheet name="EntitlementTypes" sheetId="31" r:id="rId18"/>
+    <sheet name="EntitlementStatus" sheetId="32" r:id="rId19"/>
+    <sheet name="CredentialTypes" sheetId="33" r:id="rId20"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId18"/>
+    <externalReference r:id="rId21"/>
+    <externalReference r:id="rId22"/>
   </externalReferences>
   <definedNames>
     <definedName name="_1__xlcn.WorksheetConnection_Core_Vocabularies_template.xlsxCoreVocabularies1" hidden="1">[1]!CoreVocabularies[#Data]</definedName>
     <definedName name="_2__xlcn.WorksheetConnection_Core_Vocabularies_template.xlsxRelations1" hidden="1">[1]!Relations[#Data]</definedName>
+    <definedName name="AdministrativeTeritorialUnits" localSheetId="19">[2]CoreVocabularies!#REF!</definedName>
     <definedName name="AdministrativeTeritorialUnits" localSheetId="10">[1]CoreVocabularies!#REF!</definedName>
     <definedName name="AdministrativeTeritorialUnits">[1]CoreVocabularies!#REF!</definedName>
+    <definedName name="AdminTeritorialUnits" localSheetId="19">[2]CoreVocabularies!#REF!</definedName>
     <definedName name="AdminTeritorialUnits" localSheetId="10">[1]CoreVocabularies!#REF!</definedName>
     <definedName name="AdminTeritorialUnits">[1]CoreVocabularies!#REF!</definedName>
+    <definedName name="AgentProvides" localSheetId="19">[2]CoreVocabularies!#REF!</definedName>
     <definedName name="AgentProvides" localSheetId="10">[1]CoreVocabularies!#REF!</definedName>
     <definedName name="AgentProvides">[1]CoreVocabularies!#REF!</definedName>
+    <definedName name="Concept" localSheetId="19">[2]CoreVocabularies!#REF!</definedName>
     <definedName name="Concept" localSheetId="10">[1]CoreVocabularies!#REF!</definedName>
     <definedName name="Concept">[1]CoreVocabularies!#REF!</definedName>
+    <definedName name="ContactPoint" localSheetId="19">[2]CoreVocabularies!#REF!</definedName>
     <definedName name="ContactPoint" localSheetId="10">[1]CoreVocabularies!#REF!</definedName>
     <definedName name="ContactPoint">[1]CoreVocabularies!#REF!</definedName>
+    <definedName name="Document" localSheetId="19">[2]CoreVocabularies!#REF!</definedName>
     <definedName name="Document" localSheetId="10">[1]CoreVocabularies!#REF!</definedName>
     <definedName name="Document">[1]CoreVocabularies!#REF!</definedName>
+    <definedName name="FormalFrameworkCreator" localSheetId="19">[2]CoreVocabularies!#REF!</definedName>
     <definedName name="FormalFrameworkCreator" localSheetId="10">[1]CoreVocabularies!#REF!</definedName>
     <definedName name="FormalFrameworkCreator">[1]CoreVocabularies!#REF!</definedName>
+    <definedName name="FoundationEvent" localSheetId="19">[2]CoreVocabularies!#REF!</definedName>
     <definedName name="FoundationEvent" localSheetId="10">[1]CoreVocabularies!#REF!</definedName>
     <definedName name="FoundationEvent">[1]CoreVocabularies!#REF!</definedName>
+    <definedName name="ImageObject" localSheetId="19">[2]CoreVocabularies!#REF!</definedName>
     <definedName name="ImageObject" localSheetId="10">[1]CoreVocabularies!#REF!</definedName>
     <definedName name="ImageObject">[1]CoreVocabularies!#REF!</definedName>
+    <definedName name="Input" localSheetId="19">[2]CoreVocabularies!#REF!</definedName>
     <definedName name="Input" localSheetId="10">[1]CoreVocabularies!#REF!</definedName>
     <definedName name="Input">[1]CoreVocabularies!#REF!</definedName>
+    <definedName name="InputDescription" localSheetId="19">[2]CoreVocabularies!#REF!</definedName>
     <definedName name="InputDescription" localSheetId="10">[1]CoreVocabularies!#REF!</definedName>
     <definedName name="InputDescription">[1]CoreVocabularies!#REF!</definedName>
+    <definedName name="InputName" localSheetId="19">[2]CoreVocabularies!#REF!</definedName>
     <definedName name="InputName" localSheetId="10">[1]CoreVocabularies!#REF!</definedName>
     <definedName name="InputName">[1]CoreVocabularies!#REF!</definedName>
+    <definedName name="InputType" localSheetId="19">[2]CoreVocabularies!#REF!</definedName>
     <definedName name="InputType" localSheetId="10">[1]CoreVocabularies!#REF!</definedName>
     <definedName name="InputType">[1]CoreVocabularies!#REF!</definedName>
+    <definedName name="OrganizationalUnit" localSheetId="19">[2]CoreVocabularies!#REF!</definedName>
     <definedName name="OrganizationalUnit" localSheetId="10">[1]CoreVocabularies!#REF!</definedName>
     <definedName name="OrganizationalUnit">[1]CoreVocabularies!#REF!</definedName>
+    <definedName name="PublicServiceHasChannel" localSheetId="19">[2]CoreVocabularies!#REF!</definedName>
     <definedName name="PublicServiceHasChannel" localSheetId="10">[1]CoreVocabularies!#REF!</definedName>
     <definedName name="PublicServiceHasChannel">[1]CoreVocabularies!#REF!</definedName>
+    <definedName name="PublicServiceHasInput" localSheetId="19">[2]CoreVocabularies!#REF!</definedName>
     <definedName name="PublicServiceHasInput" localSheetId="10">[1]CoreVocabularies!#REF!</definedName>
     <definedName name="PublicServiceHasInput">[1]CoreVocabularies!#REF!</definedName>
+    <definedName name="PublicServiceHomepage" localSheetId="19">[2]CoreVocabularies!#REF!</definedName>
     <definedName name="PublicServiceHomepage" localSheetId="10">[1]CoreVocabularies!#REF!</definedName>
     <definedName name="PublicServiceHomepage">[1]CoreVocabularies!#REF!</definedName>
+    <definedName name="PublicServicePhysicallyAvailableAt" localSheetId="19">[2]CoreVocabularies!#REF!</definedName>
     <definedName name="PublicServicePhysicallyAvailableAt" localSheetId="10">[1]CoreVocabularies!#REF!</definedName>
     <definedName name="PublicServicePhysicallyAvailableAt">[1]CoreVocabularies!#REF!</definedName>
+    <definedName name="RuleCreator" localSheetId="19">[2]CoreVocabularies!#REF!</definedName>
     <definedName name="RuleCreator" localSheetId="10">[1]CoreVocabularies!#REF!</definedName>
     <definedName name="RuleCreator">[1]CoreVocabularies!#REF!</definedName>
   </definedNames>
@@ -110,7 +133,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="338">
   <si>
     <t>Class</t>
   </si>
@@ -283,15 +306,6 @@
     <t>Europass Standard List Of Learning Activity Types</t>
   </si>
   <si>
-    <t>http://data.europa.eu/europass/learningActivityType/educationalProgram</t>
-  </si>
-  <si>
-    <t>educational program</t>
-  </si>
-  <si>
-    <t>http://data.europa.eu/europass/learningActivityType/workShop</t>
-  </si>
-  <si>
     <t>http://data.europa.eu/europass/learningActivityType/internship</t>
   </si>
   <si>
@@ -310,12 +324,6 @@
     <t>Europass Standard List Of Assessment Types</t>
   </si>
   <si>
-    <t>http://data.europa.eu/europass/assessmentType/writtenExamen</t>
-  </si>
-  <si>
-    <t>http://data.europa.eu/europass/assessmentType/oralExamen</t>
-  </si>
-  <si>
     <t>http://data.europa.eu/europass/assessmentType/continuousEvaluation</t>
   </si>
   <si>
@@ -358,9 +366,6 @@
     <t>self-motivated study</t>
   </si>
   <si>
-    <t>http://data.europa.eu/europass/learningActivityType/selfmotivatedstudy</t>
-  </si>
-  <si>
     <t>volunteering</t>
   </si>
   <si>
@@ -370,9 +375,6 @@
     <t>job experience</t>
   </si>
   <si>
-    <t>http://data.europa.eu/europass/learningActivityType/jobexperience</t>
-  </si>
-  <si>
     <t>classroom coursework</t>
   </si>
   <si>
@@ -400,42 +402,18 @@
     <t>written examination</t>
   </si>
   <si>
-    <t>supervised written examination</t>
-  </si>
-  <si>
     <t>oral examination</t>
   </si>
   <si>
-    <t>supervised oral examination</t>
-  </si>
-  <si>
     <t>marked assignment</t>
   </si>
   <si>
     <t>http://data.europa.eu/europass/assessmentType/markedAssignment</t>
   </si>
   <si>
-    <t>marking of an assignment</t>
-  </si>
-  <si>
-    <t>evaluation based on observation of activities</t>
-  </si>
-  <si>
-    <t>Europass Standard List of Modes Of Learning and Assessment.</t>
-  </si>
-  <si>
-    <t>Europass Standard List of Learning Opportunity Types.</t>
-  </si>
-  <si>
-    <t>Europass Standard List of Communication Channel Types.</t>
-  </si>
-  <si>
     <t>Europass Standard List of Learning Setting Types</t>
   </si>
   <si>
-    <t>Europass Standard List of Educational Credit Systems.</t>
-  </si>
-  <si>
     <t>Europass Standard List of Accreditation Types</t>
   </si>
   <si>
@@ -493,12 +471,6 @@
     <t>Europass Standard List of Target Groups</t>
   </si>
   <si>
-    <t>http://data.europa.eu/europass/targetGroup/adults</t>
-  </si>
-  <si>
-    <t>Adult education</t>
-  </si>
-  <si>
     <t>http://data.europa.eu/europass/codeList/modesOfLearningAndAssessment</t>
   </si>
   <si>
@@ -523,15 +495,9 @@
     <t>Course</t>
   </si>
   <si>
-    <t>Europass Standard List of Learning Schedule Types.</t>
-  </si>
-  <si>
     <t>http://data.europa.eu/europass/codeList/learningScheduleTypes</t>
   </si>
   <si>
-    <t>Europass Standard List of Target Groups.</t>
-  </si>
-  <si>
     <t>Part time intensive (8 to 30 hours)</t>
   </si>
   <si>
@@ -547,15 +513,6 @@
     <t xml:space="preserve">Part time intensive </t>
   </si>
   <si>
-    <t>PT light</t>
-  </si>
-  <si>
-    <t>http://data.europa.eu/europass/learningOpportunityType/educationalProgram</t>
-  </si>
-  <si>
-    <t>http://data.europa.eu/europass/learningOpportunityType/programModule</t>
-  </si>
-  <si>
     <t>http://data.europa.eu/europass/learningOpportunityType/course</t>
   </si>
   <si>
@@ -565,12 +522,6 @@
     <t>http://data.europa.eu/europass/learningOpportunityType/thesis</t>
   </si>
   <si>
-    <t>Educational program</t>
-  </si>
-  <si>
-    <t>Program module</t>
-  </si>
-  <si>
     <t>Thesis</t>
   </si>
   <si>
@@ -637,9 +588,6 @@
     <t>http://data.europa.eu/europass/methodOfSupervisionAndVerification/unsupervisedWithIDVerification</t>
   </si>
   <si>
-    <t>http://data.europa.eu/europass/communicationChannelType/mobilephone</t>
-  </si>
-  <si>
     <t>http://data.europa.eu/europass/communicationChannelType/email</t>
   </si>
   <si>
@@ -685,9 +633,6 @@
     <t>ESCO skossified version</t>
   </si>
   <si>
-    <t>Europass Standard List of Verification Types.</t>
-  </si>
-  <si>
     <t>Europass Standard List of Verification Statusses</t>
   </si>
   <si>
@@ -740,13 +685,510 @@
   </si>
   <si>
     <t>revocation</t>
+  </si>
+  <si>
+    <t>Europass Standard List of Entitlement Types</t>
+  </si>
+  <si>
+    <t>Europass Standard List of Entitlement Status</t>
+  </si>
+  <si>
+    <t>http://data.europa.eu/europass/codeList/entitlementTypes</t>
+  </si>
+  <si>
+    <t>http://data.europa.eu/europass/entitlementType/membership</t>
+  </si>
+  <si>
+    <t>http://data.europa.eu/europass/entitlementType/occupation</t>
+  </si>
+  <si>
+    <t>http://data.europa.eu/europass/entitlementType/learningOpportunity</t>
+  </si>
+  <si>
+    <t>membership</t>
+  </si>
+  <si>
+    <t>occupation</t>
+  </si>
+  <si>
+    <t>learningOpportunity</t>
+  </si>
+  <si>
+    <t>http://data.europa.eu/europass/codeList/entitlementStatuses</t>
+  </si>
+  <si>
+    <t>Europass Standard List of Entitlement Statuses</t>
+  </si>
+  <si>
+    <t>http://data.europa.eu/europass/entitlementStatus/prospective</t>
+  </si>
+  <si>
+    <t>http://data.europa.eu/europass/entitlementStatus/actual</t>
+  </si>
+  <si>
+    <t>prospective</t>
+  </si>
+  <si>
+    <t>actual</t>
+  </si>
+  <si>
+    <t>Persons who have completed primary education</t>
+  </si>
+  <si>
+    <t>Persons who have completed secondary/compulsory education</t>
+  </si>
+  <si>
+    <t>Persons who have completed tertiary education (EQF 6)</t>
+  </si>
+  <si>
+    <t>Persons who have completed tertiary education (EQF 7)</t>
+  </si>
+  <si>
+    <t>Persons who have completed tertiary education (EQF 8)</t>
+  </si>
+  <si>
+    <t>Persons in primary education</t>
+  </si>
+  <si>
+    <t>Persons in secondary/compulsory education</t>
+  </si>
+  <si>
+    <t>Persons in tertiary education (EQF 7)</t>
+  </si>
+  <si>
+    <t>Persons in tertiary education (EQF 8)</t>
+  </si>
+  <si>
+    <t>Low Achievers</t>
+  </si>
+  <si>
+    <t>High Achievers</t>
+  </si>
+  <si>
+    <t>Migrants</t>
+  </si>
+  <si>
+    <t>Persons with a learning disability</t>
+  </si>
+  <si>
+    <t>Native Speakers</t>
+  </si>
+  <si>
+    <t>Non-Native Speakers</t>
+  </si>
+  <si>
+    <t>Persons requiring employment retraining</t>
+  </si>
+  <si>
+    <t>Part time light</t>
+  </si>
+  <si>
+    <t>FF</t>
+  </si>
+  <si>
+    <t>PT</t>
+  </si>
+  <si>
+    <t>PTL</t>
+  </si>
+  <si>
+    <t>A quality assurance procedure applied at the level of an organisation. Institutional Quality Assurance leads to a QA Decision, but does not have any legal implications. Institutional Quality Assurance may be provided within the context of private QA labels.</t>
+  </si>
+  <si>
+    <t>A quality assurance procedure applied at the level of one or several programmes. Programme Quality Assurance leads to a QA Decision, but does not have any legal implications. Programme Quality Assurance may be given within the context of private QA labels.</t>
+  </si>
+  <si>
+    <t>A licencing procedure applied at the level of an organisation. Institutional Licencing implies permission for the institution to operate, and is awarded by Public Authorities or delegates thereof.</t>
+  </si>
+  <si>
+    <t>A licencing procedure applied at the level of one or several programmes. Institutional Licencing implies permission for an  institution to provide a specific programme, and is awarded by Public Authorities or delegates thereof.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check whether the the person presenting the credential is the owner. Includes:
+(a)	Comparison of  the Name and Date of Birth written in the credential with the name and date of birth stored in a person’s national eID. </t>
+  </si>
+  <si>
+    <t>http://data.europa.eu/europass/verificationType/accreditation</t>
+  </si>
+  <si>
+    <t>Check whether the the credential has been revoked. Includes:
+(a)	check if revocation certificate has been published to address indicated in the credential.
+(b)	Check if revocation certificate has been published to national revocation list
+(c)	Check if revocation certificate has been published to EU revocation list</t>
+  </si>
+  <si>
+    <t>accreditation</t>
+  </si>
+  <si>
+    <t>Check whether the awarding body is authorised to issue the credential. Includes:
+(a)	check if credential is an NQF qualification award.
+(b)	If it is, check that institution or qualification is in the accreditation database by comparing UID of qualification and/or institution with that in the accreditation database</t>
+  </si>
+  <si>
+    <t>http://data.europa.eu/europass/verificationType/expiry</t>
+  </si>
+  <si>
+    <t>validity</t>
+  </si>
+  <si>
+    <t>expiry</t>
+  </si>
+  <si>
+    <t>Check whether the credential is still valid. Includes:
+(a) check against expiry information contained with credential</t>
+  </si>
+  <si>
+    <t>An actual entitlement grants the right to pursue a learning opportunity, employment or membership automatically.</t>
+  </si>
+  <si>
+    <t>Europass Standard List of Learning Schedule Types</t>
+  </si>
+  <si>
+    <t>Europass Standard List of Learning Opportunity Types</t>
+  </si>
+  <si>
+    <t>Europass Standard List of Modes Of Learning and Assessment</t>
+  </si>
+  <si>
+    <t>Europass Standard List of Educational Credit Systems</t>
+  </si>
+  <si>
+    <t>Europass Standard List of Communication Channel Types</t>
+  </si>
+  <si>
+    <t>Europass Standard List of Communication Channel Usage Types</t>
+  </si>
+  <si>
+    <t>Europass Standard List of Skill Alignment Types</t>
+  </si>
+  <si>
+    <t>http://data.europa.eu/europass/learningOpportunityType/educationalProgramme</t>
+  </si>
+  <si>
+    <t>Educational programme</t>
+  </si>
+  <si>
+    <t>Programme module</t>
+  </si>
+  <si>
+    <t>http://data.europa.eu/europass/learningOpportunityType/programmeModule</t>
+  </si>
+  <si>
+    <t>Apprenticeship</t>
+  </si>
+  <si>
+    <t>Study visit</t>
+  </si>
+  <si>
+    <t>http://data.europa.eu/europass/learningOpportunityType/apprenticeship</t>
+  </si>
+  <si>
+    <t>http://data.europa.eu/europass/learningOpportunityType/studyVisit</t>
+  </si>
+  <si>
+    <t>Mentoring</t>
+  </si>
+  <si>
+    <t>http://data.europa.eu/europass/learningOpportunityType/mentoring</t>
+  </si>
+  <si>
+    <t>Service learning</t>
+  </si>
+  <si>
+    <t>http://data.europa.eu/europass/learningOpportunityType/serviceLearning</t>
+  </si>
+  <si>
+    <t>Persons in tertiary education (EQF 6)</t>
+  </si>
+  <si>
+    <t>Persons with 0-3 years work experience</t>
+  </si>
+  <si>
+    <t>Persons with 10+ years work experience</t>
+  </si>
+  <si>
+    <t>Persons with 3-10 years work experience</t>
+  </si>
+  <si>
+    <t>Short learning programme</t>
+  </si>
+  <si>
+    <t>MOOC</t>
+  </si>
+  <si>
+    <t>http://data.europa.eu/europass/learningOpportunityType/shortLearningProgramme</t>
+  </si>
+  <si>
+    <t>http://data.europa.eu/europass/learningOpportunityType/MOOC</t>
+  </si>
+  <si>
+    <t>Internship</t>
+  </si>
+  <si>
+    <t>http://data.europa.eu/europass/learningOpportunityType/internship</t>
+  </si>
+  <si>
+    <t>Project based</t>
+  </si>
+  <si>
+    <t>http://data.europa.eu/europass/modeOfLearningAndAssessment/projectBased</t>
+  </si>
+  <si>
+    <t>http://data.europa.eu/europass/modeOfLearningAndAssessment/laboratoryPractice</t>
+  </si>
+  <si>
+    <t>Check as to whether the credential has been issued according to the standard specified for that credential-type. Includes:
+(a)	technical check of the XML file for validity
+(b)	check if credential has basic required fields for all credentials
+(c)	check if credential has followed the rules indicated against the application profile for that specific credential-type stored at data.europa.eu</t>
+  </si>
+  <si>
+    <t>Check as to whether the credential has been tampered with. Includes:
+(a)	check that the eSeal is valid</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A prospective entitlement awards the right to </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>apply</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> for a (specific or class of) learning opportunity, employment or membership.</t>
+    </r>
+  </si>
+  <si>
+    <t>Where is this tab?</t>
+  </si>
+  <si>
+    <t>educational programme</t>
+  </si>
+  <si>
+    <t>http://data.europa.eu/europass/learningActivityType/educationalProgramme</t>
+  </si>
+  <si>
+    <t>http://data.europa.eu/europass/learningActivityType/workshop</t>
+  </si>
+  <si>
+    <t>http://data.europa.eu/europass/learningActivityType/selfMotivatedStudy</t>
+  </si>
+  <si>
+    <t>http://data.europa.eu/europass/learningActivityType/jobExperience</t>
+  </si>
+  <si>
+    <t>Learning which takes place through planned activities (in terms of learning objectives, learning time) where some form of learning support is present (e.g. student-teacher relationships); it may cover programmes to impart work skills, adult literacy and basic education for early school leavers; very common cases of non-formal learning include in-company training, through which companies update and improve the skills of their workers such as ICT skills, structured on-line learning (e.g. by making use of open educational resources), and courses
+organised by civil society organisations for their members, their target group or the general public.</t>
+  </si>
+  <si>
+    <t>Learning which takes place in an organised and structured environment, specifically dedicated to learning, and typically leads to the award of a qualification, usually in the form of a certificate or a diploma; it includes systems of general education, initial vocational training and higher education.</t>
+  </si>
+  <si>
+    <t>http://data.europa.eu/europass/assessmentType/writtenExam</t>
+  </si>
+  <si>
+    <t>http://data.europa.eu/europass/assessmentType/oralExam</t>
+  </si>
+  <si>
+    <t>peer assessment</t>
+  </si>
+  <si>
+    <t>portfolio</t>
+  </si>
+  <si>
+    <t>level of attendance</t>
+  </si>
+  <si>
+    <t>project work</t>
+  </si>
+  <si>
+    <t>group performance</t>
+  </si>
+  <si>
+    <t>practical assessment</t>
+  </si>
+  <si>
+    <t>artefact assessment</t>
+  </si>
+  <si>
+    <t>http://data.europa.eu/europass/assessmentType/peerAssessment</t>
+  </si>
+  <si>
+    <t>http://data.europa.eu/europass/assessmentType/portfolio</t>
+  </si>
+  <si>
+    <t>http://data.europa.eu/europass/assessmentType/attendance</t>
+  </si>
+  <si>
+    <t>http://data.europa.eu/europass/assessmentType/project</t>
+  </si>
+  <si>
+    <t>http://data.europa.eu/europass/assessmentType/groupPerformance</t>
+  </si>
+  <si>
+    <t>http://data.europa.eu/europass/assessmentType/practical</t>
+  </si>
+  <si>
+    <t>http://data.europa.eu/europass/assessmentType/artefact</t>
+  </si>
+  <si>
+    <t>http://data.europa.eu/europass/communicationChannelType/mobilePhone</t>
+  </si>
+  <si>
+    <t>http://data.europa.eu/europass/communicationChannelUsage/legal</t>
+  </si>
+  <si>
+    <t>Research-Lab based</t>
+  </si>
+  <si>
+    <t>http://data.europa.eu/europass/targetGroup/completedprimary</t>
+  </si>
+  <si>
+    <t>http://data.europa.eu/europass/targetGroup/completedcompulsory</t>
+  </si>
+  <si>
+    <t>http://data.europa.eu/europass/targetGroup/completedEQF6</t>
+  </si>
+  <si>
+    <t>http://data.europa.eu/europass/targetGroup/completedEQF7</t>
+  </si>
+  <si>
+    <t>http://data.europa.eu/europass/targetGroup/completedEQF8</t>
+  </si>
+  <si>
+    <t>http://data.europa.eu/europass/targetGroup/inprimary</t>
+  </si>
+  <si>
+    <t>http://data.europa.eu/europass/targetGroup/incompulsory</t>
+  </si>
+  <si>
+    <t>http://data.europa.eu/europass/targetGroup/inEQF6</t>
+  </si>
+  <si>
+    <t>http://data.europa.eu/europass/targetGroup/inEQF7</t>
+  </si>
+  <si>
+    <t>http://data.europa.eu/europass/targetGroup/inEQF8</t>
+  </si>
+  <si>
+    <t>http://data.europa.eu/europass/targetGroup/3yearwork</t>
+  </si>
+  <si>
+    <t>http://data.europa.eu/europass/targetGroup/0yearwork</t>
+  </si>
+  <si>
+    <t>http://data.europa.eu/europass/targetGroup/10yearwork</t>
+  </si>
+  <si>
+    <t>http://data.europa.eu/europass/targetGroup/requireretraining</t>
+  </si>
+  <si>
+    <t>http://data.europa.eu/europass/targetGroup/lowachievers</t>
+  </si>
+  <si>
+    <t>http://data.europa.eu/europass/targetGroup/highachievers</t>
+  </si>
+  <si>
+    <t>http://data.europa.eu/europass/targetGroup/migrants</t>
+  </si>
+  <si>
+    <t>http://data.europa.eu/europass/targetGroup/learningdisability</t>
+  </si>
+  <si>
+    <t>http://data.europa.eu/europass/targetGroup/nativespeakers</t>
+  </si>
+  <si>
+    <t>http://data.europa.eu/europass/targetGroup/nonnativespeakers</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>Fax</t>
+  </si>
+  <si>
+    <t>Web</t>
+  </si>
+  <si>
+    <t>Post</t>
+  </si>
+  <si>
+    <t>Mobile Phone</t>
+  </si>
+  <si>
+    <t>E-Mail</t>
+  </si>
+  <si>
+    <t>Personal</t>
+  </si>
+  <si>
+    <t>Business</t>
+  </si>
+  <si>
+    <t>Mobile</t>
+  </si>
+  <si>
+    <t>Legal</t>
+  </si>
+  <si>
+    <t>learning Opportunity</t>
+  </si>
+  <si>
+    <t>http://data.europa.eu/europass/codeList/credentialTypes</t>
+  </si>
+  <si>
+    <t>Europass Standard List of Credential Types.</t>
+  </si>
+  <si>
+    <t>http://data.europa.eu/europass/credentialType/generic</t>
+  </si>
+  <si>
+    <t>generic</t>
+  </si>
+  <si>
+    <t>This is the default Europass credential type.</t>
+  </si>
+  <si>
+    <t>http://data.europa.eu/europass/credentialType/qualification</t>
+  </si>
+  <si>
+    <t>qualification award</t>
+  </si>
+  <si>
+    <t>Represents the award of a qualification by an institution that is accredited to do so, confirmed by its inclusion in the Europass Accreditation Database.</t>
+  </si>
+  <si>
+    <t>http://data.europa.eu/europass/credentialType/diplomaSupplement</t>
+  </si>
+  <si>
+    <t>diploma supplement</t>
+  </si>
+  <si>
+    <t>diplomaSupplement</t>
+  </si>
+  <si>
+    <t>Represents the award of a higher education qualification by an institution that is accredited to do so, confirmed by its inclusion in the Europass Accreditation Database, and including all diploma supplement information.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -789,8 +1231,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -812,6 +1268,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFEACA8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -844,7 +1306,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -882,6 +1344,39 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -919,6 +1414,7 @@
   </tableStyles>
   <colors>
     <mruColors>
+      <color rgb="FFFEACA8"/>
       <color rgb="FFCCECFF"/>
     </mruColors>
   </colors>
@@ -934,6 +1430,31 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="CoreVocabularies"/>
+      <sheetName val="Data Types"/>
+      <sheetName val="TargetVocabulary"/>
+      <sheetName val="Mapping"/>
+      <sheetName val="Mappings analysis"/>
+      <sheetName val="Meta-model"/>
+      <sheetName val="core_vocabularies_v2.00"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
@@ -1270,21 +1791,21 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D7C65FB-96B7-4669-B8D7-C5F8AC7942F1}">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:K40"/>
+  <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33:A34"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="65.83984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40.7890625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="57.15625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32.7890625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="65.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="57.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
         <v>5</v>
       </c>
@@ -1299,12 +1820,12 @@
       <c r="J1" s="10"/>
       <c r="K1" s="10"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="11" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" s="12" t="s">
         <v>7</v>
       </c>
@@ -1313,7 +1834,7 @@
       </c>
       <c r="D4" s="12"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" s="12" t="s">
         <v>9</v>
       </c>
@@ -1322,12 +1843,12 @@
       </c>
       <c r="D5" s="12"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" s="11" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" s="12" t="s">
         <v>12</v>
       </c>
@@ -1335,7 +1856,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="12" t="s">
         <v>14</v>
       </c>
@@ -1346,207 +1867,225 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" s="12"/>
       <c r="B10" s="12"/>
       <c r="C10" s="12"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" s="11" t="s">
         <v>17</v>
       </c>
       <c r="B11" s="12"/>
       <c r="C11" s="12"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" s="12" t="s">
         <v>18</v>
       </c>
       <c r="B12" s="12"/>
       <c r="C12" s="12"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14" s="11" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" s="16" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16" s="12" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17" s="12" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A19" s="12" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A20" s="12" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A21" s="12" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A22" s="12" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A23" s="12" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A24" s="12" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A25" s="12" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A26" s="12" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A27" s="12" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A28" s="12" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A29" s="12" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A30" s="12" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A31" s="12" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A32" s="12"/>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A33" s="11" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A32" s="12" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A33" s="12" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A34" s="12" t="s">
+        <v>239</v>
+      </c>
+      <c r="B34" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A35" s="12"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A36" s="11" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A34" s="12" t="s">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A37" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="B34" s="12" t="s">
+      <c r="B37" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="C34" s="12" t="s">
+      <c r="C37" s="12" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A35" s="12" t="s">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A38" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="B35" s="12" t="s">
+      <c r="B38" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="C35" s="12" t="s">
+      <c r="C38" s="12" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A36" s="12" t="s">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A39" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="B36" s="12" t="s">
+      <c r="B39" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="C36" s="12" t="s">
+      <c r="C39" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="D36" s="12" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A37" s="12" t="s">
+      <c r="D39" s="12" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A40" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B37" s="12" t="s">
+      <c r="B40" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="C37" s="12" t="s">
+      <c r="C40" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="D37" s="12" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A38" s="12" t="s">
+      <c r="D40" s="12" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A41" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="B38" s="12" t="s">
+      <c r="B41" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="C38" s="12" t="s">
+      <c r="C41" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="D38" s="12" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A39" s="12" t="s">
+      <c r="D41" s="12" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A42" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B39" s="12" t="s">
+      <c r="B42" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="C39" s="12" t="s">
+      <c r="C42" s="12" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A40" s="12" t="s">
-        <v>185</v>
-      </c>
-      <c r="B40" s="12" t="s">
-        <v>186</v>
-      </c>
-      <c r="C40" s="12" t="s">
-        <v>187</v>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A43" s="12" t="s">
+        <v>160</v>
+      </c>
+      <c r="B43" s="12" t="s">
+        <v>161</v>
+      </c>
+      <c r="C43" s="12" t="s">
+        <v>162</v>
       </c>
     </row>
   </sheetData>
@@ -1558,19 +2097,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8A029B5-659D-4026-951A-6E6448106C10}">
   <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.68359375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="60.89453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="45.89453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.89453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="67" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1587,7 +2126,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>45</v>
       </c>
@@ -1596,18 +2135,18 @@
       <c r="D2" s="2"/>
       <c r="E2" s="6"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="7"/>
       <c r="B3" s="7" t="s">
-        <v>181</v>
+        <v>156</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>110</v>
+        <v>95</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="4"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>47</v>
       </c>
@@ -1616,30 +2155,46 @@
       <c r="D4" s="2"/>
       <c r="E4" s="6"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="8" t="s">
         <v>48</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>182</v>
-      </c>
-      <c r="C5" s="7"/>
+        <v>157</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>321</v>
+      </c>
       <c r="D5" s="7"/>
       <c r="E5" s="4"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B6" s="7" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+        <v>158</v>
+      </c>
+      <c r="C6" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="22" spans="7:7" x14ac:dyDescent="0.55000000000000004">
+        <v>159</v>
+      </c>
+      <c r="C7" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B8" s="20" t="s">
+        <v>293</v>
+      </c>
+      <c r="C8" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="22" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G22" t="s">
-        <v>180</v>
+        <v>155</v>
       </c>
     </row>
   </sheetData>
@@ -1655,20 +2210,20 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3:E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.5234375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="59.7890625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="40.47265625" customWidth="1"/>
-    <col min="4" max="4" width="13.7890625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.5234375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="55.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="54.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1685,7 +2240,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>45</v>
       </c>
@@ -1694,7 +2249,7 @@
       <c r="D2" s="2"/>
       <c r="E2" s="6"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="7"/>
       <c r="B3" s="7" t="s">
         <v>46</v>
@@ -1705,7 +2260,7 @@
       <c r="D3" s="7"/>
       <c r="E3" s="4"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>47</v>
       </c>
@@ -1714,7 +2269,7 @@
       <c r="D4" s="2"/>
       <c r="E4" s="6"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A5" s="8" t="s">
         <v>48</v>
       </c>
@@ -1727,23 +2282,28 @@
       <c r="D5" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="E5" s="4"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="E5" s="17" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="159.5" x14ac:dyDescent="0.35">
       <c r="B6" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="7" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="E6" s="18" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B7" s="7"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B8" s="7"/>
     </row>
   </sheetData>
@@ -1757,20 +2317,20 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3:C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.5234375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="59.7890625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="40.47265625" customWidth="1"/>
-    <col min="4" max="4" width="13.7890625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.5234375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="66.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1787,7 +2347,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>45</v>
       </c>
@@ -1796,7 +2356,7 @@
       <c r="D2" s="2"/>
       <c r="E2" s="6"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="7"/>
       <c r="B3" s="7" t="s">
         <v>55</v>
@@ -1807,7 +2367,7 @@
       <c r="D3" s="7"/>
       <c r="E3" s="4"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>47</v>
       </c>
@@ -1816,108 +2376,107 @@
       <c r="D4" s="2"/>
       <c r="E4" s="6"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="8" t="s">
         <v>48</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>57</v>
+        <v>270</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>58</v>
+        <v>269</v>
       </c>
       <c r="D5" s="7"/>
       <c r="E5" s="4"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B6" s="7" t="s">
+        <v>271</v>
+      </c>
+      <c r="C6" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B7" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="C7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B8" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B9" t="s">
+        <v>272</v>
+      </c>
+      <c r="C9" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B10" t="s">
+        <v>78</v>
+      </c>
+      <c r="C10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B11" t="s">
+        <v>273</v>
+      </c>
+      <c r="C11" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B12" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="C12" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="B7" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="C7" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="B8" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="C8" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="B9" s="13" t="s">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B13" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="C13" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B14" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="C14" t="s">
         <v>82</v>
       </c>
-      <c r="C9" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="B10" t="s">
-        <v>84</v>
-      </c>
-      <c r="C10" t="s">
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B15" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="C15" t="s">
         <v>83</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="B11" t="s">
-        <v>86</v>
-      </c>
-      <c r="C11" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="B12" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="C12" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="B13" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="C13" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="B14" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="C14" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="B15" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="C15" t="s">
-        <v>90</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B9" r:id="rId1" xr:uid="{0FA044CC-23B4-479F-8B6C-0BD9A1078A16}"/>
-    <hyperlink ref="B10" r:id="rId2" xr:uid="{D94DB506-4DDC-4956-9E3A-11390C61E4D6}"/>
-    <hyperlink ref="B11" r:id="rId3" xr:uid="{0C82C18B-0A3B-456A-89D7-71CFC2AA465F}"/>
-    <hyperlink ref="B12" r:id="rId4" xr:uid="{13B7B3EE-0B4C-41B2-8949-B083D6A5C361}"/>
-    <hyperlink ref="B13" r:id="rId5" xr:uid="{AF368D94-FEA9-4FCE-88A2-4B196070ECCF}"/>
-    <hyperlink ref="B14" r:id="rId6" xr:uid="{0B9EE4A3-0928-477F-BA75-56A6AAE0D011}"/>
-    <hyperlink ref="B15" r:id="rId7" xr:uid="{67720231-91F4-4B00-B299-94BD69186D9C}"/>
+    <hyperlink ref="B10" r:id="rId1" xr:uid="{D94DB506-4DDC-4956-9E3A-11390C61E4D6}"/>
+    <hyperlink ref="B12" r:id="rId2" xr:uid="{13B7B3EE-0B4C-41B2-8949-B083D6A5C361}"/>
+    <hyperlink ref="B13" r:id="rId3" xr:uid="{AF368D94-FEA9-4FCE-88A2-4B196070ECCF}"/>
+    <hyperlink ref="B14" r:id="rId4" xr:uid="{0B9EE4A3-0928-477F-BA75-56A6AAE0D011}"/>
+    <hyperlink ref="B15" r:id="rId5" xr:uid="{67720231-91F4-4B00-B299-94BD69186D9C}"/>
+    <hyperlink ref="B11" r:id="rId6" display="http://data.europa.eu/europass/learningActivityType/jobexperience" xr:uid="{0C82C18B-0A3B-456A-89D7-71CFC2AA465F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1926,22 +2485,22 @@
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBF2179B-A626-4B01-8217-09B8759F2BAD}">
   <sheetPr codeName="Sheet7"/>
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:E5"/>
+    <sheetView topLeftCell="B7" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.47265625" style="7" customWidth="1"/>
-    <col min="2" max="2" width="57.734375" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.5234375" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.7890625" style="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="38.47265625" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.453125" style="7" customWidth="1"/>
+    <col min="2" max="2" width="62.26953125" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.26953125" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.54296875" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="38.453125" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1958,7 +2517,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>45</v>
       </c>
@@ -1967,15 +2526,15 @@
       <c r="D2" s="2"/>
       <c r="E2" s="6"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B3" s="7" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>47</v>
       </c>
@@ -1984,51 +2543,95 @@
       <c r="D4" s="2"/>
       <c r="E4" s="6"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="8" t="s">
         <v>48</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>66</v>
+        <v>276</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B6" s="7" t="s">
-        <v>67</v>
+        <v>277</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B7" s="7" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B8" s="7" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>102</v>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B9" s="7" t="s">
+        <v>285</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B10" s="7" t="s">
+        <v>286</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B11" s="7" t="s">
+        <v>287</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B12" s="7" t="s">
+        <v>288</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B13" s="7" t="s">
+        <v>289</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B14" s="7" t="s">
+        <v>290</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B15" s="7" t="s">
+        <v>291</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>284</v>
       </c>
     </row>
   </sheetData>
@@ -2045,19 +2648,19 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E5"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="31.5234375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="53.7890625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.5234375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.7890625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.5234375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="53.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2074,7 +2677,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>45</v>
       </c>
@@ -2083,10 +2686,10 @@
       <c r="D2" s="2"/>
       <c r="E2" s="6"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="7"/>
       <c r="B3" s="7" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>24</v>
@@ -2094,7 +2697,7 @@
       <c r="D3" s="7"/>
       <c r="E3" s="4"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>47</v>
       </c>
@@ -2103,52 +2706,52 @@
       <c r="D4" s="2"/>
       <c r="E4" s="6"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="8" t="s">
         <v>48</v>
       </c>
       <c r="B5" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="E5" s="4"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B6" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B7" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="C7" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="C5" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="E5" s="4"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="B6" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="B7" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>76</v>
-      </c>
       <c r="D7" s="7" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B8" s="7" t="s">
-        <v>188</v>
+        <v>163</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>189</v>
+        <v>164</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>189</v>
+        <v>164</v>
       </c>
     </row>
   </sheetData>
@@ -2168,16 +2771,16 @@
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="40.5234375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="58.7890625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="40.5234375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.7890625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.5234375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="58.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2194,7 +2797,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>45</v>
       </c>
@@ -2203,10 +2806,10 @@
       <c r="D2" s="2"/>
       <c r="E2" s="6"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="7"/>
       <c r="B3" s="13" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>25</v>
@@ -2214,7 +2817,7 @@
       <c r="D3" s="7"/>
       <c r="E3" s="4"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>47</v>
       </c>
@@ -2223,27 +2826,27 @@
       <c r="D4" s="2"/>
       <c r="E4" s="6"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="8" t="s">
         <v>48</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="E5" s="4"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
       <c r="D6" s="7"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
@@ -2258,118 +2861,159 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95D8780A-898E-42B0-8AD8-52D762622FBE}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView topLeftCell="B6" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.26171875" customWidth="1"/>
-    <col min="2" max="2" width="48.83984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.15625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.89453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.68359375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.26953125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="54.54296875" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.54296875" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.81640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="49.453125" style="4" customWidth="1"/>
+    <col min="6" max="16384" width="8.7265625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="21" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="6"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B2" s="24"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="24"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="7"/>
       <c r="B3" s="7" t="s">
-        <v>193</v>
+        <v>167</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>194</v>
+        <v>168</v>
       </c>
       <c r="D3" s="7"/>
-      <c r="E3" s="4"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="3" t="s">
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="B4" s="6"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="6"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B4" s="24"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="24"/>
+    </row>
+    <row r="5" spans="1:5" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A5" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="B5" t="s">
-        <v>196</v>
+      <c r="B5" s="4" t="s">
+        <v>170</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>206</v>
+        <v>180</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>206</v>
-      </c>
-      <c r="E5" s="4"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="B6" t="s">
-        <v>197</v>
-      </c>
-      <c r="C6" t="s">
-        <v>207</v>
-      </c>
-      <c r="D6" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="B7" t="s">
-        <v>198</v>
-      </c>
-      <c r="C7" t="s">
-        <v>208</v>
-      </c>
-      <c r="D7" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="B8" t="s">
-        <v>199</v>
-      </c>
-      <c r="C8" t="s">
-        <v>209</v>
-      </c>
-      <c r="D8" t="s">
-        <v>209</v>
+        <v>180</v>
+      </c>
+      <c r="E5" s="17" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B6" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="E6" s="17" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="B7" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="E7" s="17" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="116" x14ac:dyDescent="0.35">
+      <c r="B8" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="E8" s="17" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="87" x14ac:dyDescent="0.35">
+      <c r="B9" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="E9" s="17" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B10" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="E10" s="17" t="s">
+        <v>231</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1" xr:uid="{23B72603-5D70-4560-A169-4FE75E51A07B}"/>
+    <hyperlink ref="B9" r:id="rId2" xr:uid="{CC5F6694-0DA5-4A86-8633-C25E6FBF922E}"/>
+    <hyperlink ref="B10" r:id="rId3" display="http://data.europa.eu/europass/verificationType/accreditation" xr:uid="{83B6978E-52B1-4E3E-9D5F-E02BD79032AF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2380,19 +3024,19 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.68359375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="50.41796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="37.9453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.89453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.68359375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="54.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2409,7 +3053,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>45</v>
       </c>
@@ -2418,18 +3062,18 @@
       <c r="D2" s="2"/>
       <c r="E2" s="6"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="7"/>
       <c r="B3" t="s">
-        <v>195</v>
+        <v>169</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>192</v>
+        <v>166</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="4"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>47</v>
       </c>
@@ -2438,46 +3082,259 @@
       <c r="D4" s="2"/>
       <c r="E4" s="6"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="8" t="s">
         <v>48</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>200</v>
+        <v>174</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>203</v>
+        <v>177</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>203</v>
+        <v>177</v>
       </c>
       <c r="E5" s="4"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
-        <v>201</v>
+        <v>175</v>
       </c>
       <c r="C6" t="s">
-        <v>204</v>
+        <v>178</v>
       </c>
       <c r="D6" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
-        <v>202</v>
+        <v>176</v>
       </c>
       <c r="C7" t="s">
-        <v>205</v>
+        <v>179</v>
       </c>
       <c r="D7" t="s">
-        <v>205</v>
+        <v>179</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1" xr:uid="{D7BF9801-1BBA-418B-842F-3D17F63ECAAB}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60F375BA-C3E0-4CF6-A95E-6FEC83A2D5A9}">
+  <dimension ref="A1:E7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="61.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.54296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" s="6"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="6"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" s="7"/>
+      <c r="B3" s="14" t="s">
+        <v>186</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="D3" s="7"/>
+      <c r="E3" s="4"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" s="6"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="6"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>187</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="E5" s="4"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B6" s="14" t="s">
+        <v>188</v>
+      </c>
+      <c r="C6" t="s">
+        <v>191</v>
+      </c>
+      <c r="D6" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B7" s="14" t="s">
+        <v>189</v>
+      </c>
+      <c r="C7" t="s">
+        <v>325</v>
+      </c>
+      <c r="D7" t="s">
+        <v>192</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B5" r:id="rId1" xr:uid="{49DFCD87-7834-43CC-B79E-2B9FCB24A423}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C8E7E74-3278-4B2F-B5AD-D784A53185A1}">
+  <dimension ref="A1:F14"/>
+  <sheetViews>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="54.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="110" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" s="6"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="6"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" s="7"/>
+      <c r="B3" t="s">
+        <v>193</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="D3" s="7"/>
+      <c r="E3" s="4"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" s="6"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="6"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B6" t="s">
+        <v>196</v>
+      </c>
+      <c r="C6" t="s">
+        <v>198</v>
+      </c>
+      <c r="D6" t="s">
+        <v>198</v>
+      </c>
+      <c r="E6" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F14" s="4"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{75A1B571-7C04-44A3-AE36-7741303B915B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2488,19 +3345,19 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="E1" sqref="C1:E1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.68359375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="59.3125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="43.47265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.3671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.81640625" customWidth="1"/>
+    <col min="2" max="2" width="66" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2517,27 +3374,25 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="2"/>
+      <c r="B2" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>233</v>
+      </c>
       <c r="D2" s="2"/>
       <c r="E2" s="6"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="7"/>
-      <c r="B3" s="14" t="s">
-        <v>138</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>137</v>
-      </c>
       <c r="D3" s="7"/>
       <c r="E3" s="4"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>47</v>
       </c>
@@ -2546,41 +3401,49 @@
       <c r="D4" s="2"/>
       <c r="E4" s="6"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="8" t="s">
         <v>48</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>168</v>
+        <v>144</v>
       </c>
       <c r="C5" t="s">
-        <v>143</v>
-      </c>
-      <c r="D5" s="7"/>
+        <v>124</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>216</v>
+      </c>
       <c r="E5" s="4" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B6" s="14" t="s">
-        <v>169</v>
+        <v>145</v>
       </c>
       <c r="C6" t="s">
-        <v>144</v>
+        <v>125</v>
+      </c>
+      <c r="D6" t="s">
+        <v>217</v>
       </c>
       <c r="E6" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B7" s="14" t="s">
-        <v>170</v>
+        <v>146</v>
       </c>
       <c r="C7" t="s">
-        <v>145</v>
+        <v>215</v>
+      </c>
+      <c r="D7" t="s">
+        <v>218</v>
       </c>
       <c r="E7" t="s">
-        <v>141</v>
+        <v>122</v>
       </c>
     </row>
   </sheetData>
@@ -2593,23 +3456,24 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE83B8A2-8B14-49F5-ADCB-B156B8F36656}">
-  <dimension ref="A1:E9"/>
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8BE5540-6620-4F6A-B713-B839A2E94AC4}">
+  <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="63.7890625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="49.68359375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.3671875" customWidth="1"/>
-    <col min="5" max="5" width="11" customWidth="1"/>
+    <col min="1" max="1" width="34.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="55.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="190.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2626,7 +3490,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>45</v>
       </c>
@@ -2635,18 +3499,18 @@
       <c r="D2" s="2"/>
       <c r="E2" s="6"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="7"/>
-      <c r="B3" s="14" t="s">
-        <v>135</v>
+      <c r="B3" t="s">
+        <v>326</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>104</v>
+        <v>327</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="4"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>47</v>
       </c>
@@ -2655,79 +3519,273 @@
       <c r="D4" s="2"/>
       <c r="E4" s="6"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="8" t="s">
         <v>48</v>
       </c>
+      <c r="B5" t="s">
+        <v>328</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>329</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>329</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B6" t="s">
+        <v>331</v>
+      </c>
+      <c r="C6" t="s">
+        <v>332</v>
+      </c>
+      <c r="D6" t="s">
+        <v>332</v>
+      </c>
+      <c r="E6" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B7" t="s">
+        <v>334</v>
+      </c>
+      <c r="C7" t="s">
+        <v>335</v>
+      </c>
+      <c r="D7" t="s">
+        <v>336</v>
+      </c>
+      <c r="E7" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A20" s="29"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{C8F2EFAA-B7AB-4A37-8DA8-3D62013978D7}"/>
+    <hyperlink ref="B5" r:id="rId2" xr:uid="{9C258BDC-28D8-4A79-8FE4-7C9E69B24C29}"/>
+    <hyperlink ref="B6" r:id="rId3" xr:uid="{E6ECDA16-62DC-4028-B517-1937DC3C79B0}"/>
+    <hyperlink ref="B7" r:id="rId4" xr:uid="{8079F9DE-1A88-4EFF-863B-87AEA290DEA2}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE83B8A2-8B14-49F5-ADCB-B156B8F36656}">
+  <dimension ref="A1:E19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:E16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="72.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.453125" customWidth="1"/>
+    <col min="5" max="5" width="11" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" s="6"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="6"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" s="7"/>
+      <c r="B3" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>234</v>
+      </c>
+      <c r="D3" s="7"/>
+      <c r="E3" s="4"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" s="6"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="6"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" s="8" t="s">
+        <v>48</v>
+      </c>
       <c r="B5" s="14" t="s">
-        <v>146</v>
-      </c>
-      <c r="C5" t="s">
-        <v>151</v>
+        <v>240</v>
+      </c>
+      <c r="C5" s="27" t="s">
+        <v>241</v>
       </c>
       <c r="D5" s="7"/>
       <c r="E5" s="4"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B6" s="14" t="s">
-        <v>147</v>
+        <v>243</v>
       </c>
       <c r="C6" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B7" s="14" t="s">
-        <v>148</v>
+        <v>126</v>
       </c>
       <c r="C7" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B8" s="14" t="s">
-        <v>149</v>
+        <v>127</v>
       </c>
       <c r="C8" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B9" s="14" t="s">
-        <v>150</v>
+        <v>128</v>
       </c>
       <c r="C9" t="s">
-        <v>153</v>
-      </c>
+        <v>129</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B10" s="14" t="s">
+        <v>246</v>
+      </c>
+      <c r="C10" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B11" s="14" t="s">
+        <v>261</v>
+      </c>
+      <c r="C11" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B12" s="14" t="s">
+        <v>247</v>
+      </c>
+      <c r="C12" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B13" s="14" t="s">
+        <v>249</v>
+      </c>
+      <c r="C13" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B14" s="14" t="s">
+        <v>251</v>
+      </c>
+      <c r="C14" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B15" s="14" t="s">
+        <v>258</v>
+      </c>
+      <c r="C15" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B16" s="14" t="s">
+        <v>259</v>
+      </c>
+      <c r="C16" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B17" s="14"/>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B18" s="14"/>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B19" s="14"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B7" r:id="rId1" xr:uid="{FDB6CB86-BD5F-4C88-91AA-A51FA39B16C2}"/>
     <hyperlink ref="B8" r:id="rId2" xr:uid="{6D7314CE-36FA-4C63-B496-9A64A6836A51}"/>
     <hyperlink ref="B9" r:id="rId3" xr:uid="{3B72C526-72C2-498F-9EC0-E018CFF6E68B}"/>
+    <hyperlink ref="B10" r:id="rId4" display="http://data.europa.eu/europass/learningOpportunityType/thesis" xr:uid="{628087DA-9187-4CAE-A646-117301D45E58}"/>
+    <hyperlink ref="B12" r:id="rId5" display="http://data.europa.eu/europass/learningOpportunityType/thesis" xr:uid="{EBE8AAB4-C4F0-4FF9-8CFD-2D5080108A92}"/>
+    <hyperlink ref="B13" r:id="rId6" display="http://data.europa.eu/europass/learningOpportunityType/thesis" xr:uid="{30D6FBA6-D76E-4B68-83DF-09F6B3C80CA6}"/>
+    <hyperlink ref="B14" r:id="rId7" display="http://data.europa.eu/europass/learningOpportunityType/thesis" xr:uid="{312DF105-B04E-4967-ABCA-682AD6D51B23}"/>
+    <hyperlink ref="B15" r:id="rId8" display="http://data.europa.eu/europass/learningOpportunityType/thesis" xr:uid="{37B9C397-63B0-466C-87D3-DAC8AD7854CA}"/>
+    <hyperlink ref="B16" r:id="rId9" display="http://data.europa.eu/europass/learningOpportunityType/thesis" xr:uid="{F74AF2FC-7DF6-4E95-9400-5883A7B68102}"/>
+    <hyperlink ref="B11" r:id="rId10" display="http://data.europa.eu/europass/learningOpportunityType/thesis" xr:uid="{9F0B96FD-F3E9-4694-BA86-66FE7009CE2B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId11"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36E16047-0E1D-4862-BB2F-84ED965D8F43}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C2" sqref="C2:E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.68359375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="62.1015625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="49.68359375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.3671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="73.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="52.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.453125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2744,7 +3802,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>45</v>
       </c>
@@ -2753,18 +3811,18 @@
       <c r="D2" s="2"/>
       <c r="E2" s="6"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="7"/>
       <c r="B3" s="14" t="s">
-        <v>129</v>
+        <v>112</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>103</v>
+        <v>235</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="4"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>47</v>
       </c>
@@ -2773,41 +3831,57 @@
       <c r="D4" s="2"/>
       <c r="E4" s="6"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="8" t="s">
         <v>48</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>131</v>
+        <v>114</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>130</v>
+        <v>113</v>
       </c>
       <c r="D5" s="7"/>
       <c r="E5" s="4"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B6" s="14" t="s">
-        <v>154</v>
+        <v>130</v>
       </c>
       <c r="C6" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B7" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="C7" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B8" s="14" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="B7" s="14" t="s">
-        <v>155</v>
-      </c>
-      <c r="C7" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="B8" s="14" t="s">
-        <v>156</v>
-      </c>
-      <c r="C8" t="s">
-        <v>134</v>
+      <c r="C8" s="7" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B9" s="14" t="s">
+        <v>263</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B10" s="14" t="s">
+        <v>264</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>294</v>
       </c>
     </row>
   </sheetData>
@@ -2816,6 +3890,8 @@
     <hyperlink ref="B6" r:id="rId2" xr:uid="{5113F2D0-C9E6-415C-BAA4-50DD12DF8F9E}"/>
     <hyperlink ref="B7" r:id="rId3" xr:uid="{911B9D20-BF7F-4623-8A76-2B3231CCE0A4}"/>
     <hyperlink ref="B8" r:id="rId4" xr:uid="{716DB0E5-1F10-418F-9E84-076D08BC3A92}"/>
+    <hyperlink ref="B9" r:id="rId5" display="http://data.europa.eu/europass/modeOfLearningAndAssessment/workbased" xr:uid="{01AD09C9-C7D5-4D81-9E1D-41B85DC77C36}"/>
+    <hyperlink ref="B10" r:id="rId6" display="http://data.europa.eu/europass/modeOfLearningAndAssessment/workbased" xr:uid="{3B904906-DF56-4116-9AAD-0FBB0FCEA340}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2823,22 +3899,22 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66DF261F-9DA6-471B-82C7-B9CFAB2AFD62}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.68359375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="68.1015625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="53.26171875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.3671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="68.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="54.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.453125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2855,7 +3931,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>45</v>
       </c>
@@ -2864,18 +3940,18 @@
       <c r="D2" s="2"/>
       <c r="E2" s="6"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="7"/>
       <c r="B3" s="14" t="s">
-        <v>125</v>
+        <v>110</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>126</v>
+        <v>111</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="4"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>47</v>
       </c>
@@ -2884,20 +3960,195 @@
       <c r="D4" s="2"/>
       <c r="E4" s="6"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="B5" s="14" t="s">
-        <v>127</v>
+      <c r="B5" s="28" t="s">
+        <v>295</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>128</v>
+        <v>199</v>
       </c>
       <c r="D5" s="7"/>
       <c r="E5" s="4"/>
     </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B6" s="28" t="s">
+        <v>296</v>
+      </c>
+      <c r="C6" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B7" s="28" t="s">
+        <v>297</v>
+      </c>
+      <c r="C7" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B8" s="28" t="s">
+        <v>298</v>
+      </c>
+      <c r="C8" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B9" s="28" t="s">
+        <v>299</v>
+      </c>
+      <c r="C9" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B10" s="28" t="s">
+        <v>300</v>
+      </c>
+      <c r="C10" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B11" s="28" t="s">
+        <v>301</v>
+      </c>
+      <c r="C11" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B12" s="28" t="s">
+        <v>302</v>
+      </c>
+      <c r="C12" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B13" s="28" t="s">
+        <v>303</v>
+      </c>
+      <c r="C13" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B14" s="28" t="s">
+        <v>304</v>
+      </c>
+      <c r="C14" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B15" s="28" t="s">
+        <v>306</v>
+      </c>
+      <c r="C15" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B16" s="28" t="s">
+        <v>305</v>
+      </c>
+      <c r="C16" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B17" s="28" t="s">
+        <v>307</v>
+      </c>
+      <c r="C17" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B18" s="28" t="s">
+        <v>308</v>
+      </c>
+      <c r="C18" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B19" s="28" t="s">
+        <v>309</v>
+      </c>
+      <c r="C19" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B20" s="28" t="s">
+        <v>310</v>
+      </c>
+      <c r="C20" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B21" s="28" t="s">
+        <v>311</v>
+      </c>
+      <c r="C21" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B22" s="28" t="s">
+        <v>312</v>
+      </c>
+      <c r="C22" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B23" s="28" t="s">
+        <v>313</v>
+      </c>
+      <c r="C23" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B24" s="28" t="s">
+        <v>314</v>
+      </c>
+      <c r="C24" t="s">
+        <v>213</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B5" r:id="rId1" xr:uid="{D56FFFD4-69C6-4B8A-856B-EEA566B823A7}"/>
+    <hyperlink ref="B6" r:id="rId2" xr:uid="{25D062AC-212F-493B-90D4-00F783B9A8AC}"/>
+    <hyperlink ref="B7" r:id="rId3" xr:uid="{33D56EEE-7BBF-43CE-982A-6A05211D287A}"/>
+    <hyperlink ref="B8" r:id="rId4" xr:uid="{CB4B4966-004A-4CD8-AEB0-042397048CF8}"/>
+    <hyperlink ref="B9" r:id="rId5" xr:uid="{965B8FF9-E390-4F65-BC08-4029FF83CD8F}"/>
+    <hyperlink ref="B10" r:id="rId6" display="http://data.europa.eu/europass/targetGroup/completedprimary" xr:uid="{C300AE65-5EC4-49D4-AB3D-F94A47B3FBFA}"/>
+    <hyperlink ref="B11" r:id="rId7" display="http://data.europa.eu/europass/targetGroup/completedcompulsory" xr:uid="{9B1F90A5-3ABA-429A-883B-82833D38AA59}"/>
+    <hyperlink ref="B12" r:id="rId8" display="http://data.europa.eu/europass/targetGroup/completedEQF6" xr:uid="{3049F4F6-E193-4DD8-BE96-3AE9CA3EB3D8}"/>
+    <hyperlink ref="B13" r:id="rId9" display="http://data.europa.eu/europass/targetGroup/completedEQF7" xr:uid="{1F281C6A-C922-460A-8F00-58CE71F91AA2}"/>
+    <hyperlink ref="B14" r:id="rId10" display="http://data.europa.eu/europass/targetGroup/completedEQF8" xr:uid="{21DCF89F-4AAB-4985-A47F-982407BF1991}"/>
+    <hyperlink ref="B15" r:id="rId11" xr:uid="{E66B5EE2-64C2-4988-BEC4-AEB216E8B478}"/>
+    <hyperlink ref="B16" r:id="rId12" xr:uid="{503DFD79-22AE-4647-B1B2-1BB19A9252D6}"/>
+    <hyperlink ref="B17" r:id="rId13" xr:uid="{CE0734A3-BA42-48AF-852F-5763CA0B5DCC}"/>
+    <hyperlink ref="B18" r:id="rId14" xr:uid="{78A2A312-3929-4DF6-9FC5-BADBC4C42419}"/>
+    <hyperlink ref="B19:B24" r:id="rId15" display="http://data.europa.eu/europass/targetGroup/requireretraining" xr:uid="{809FDF1E-829C-4161-8B9E-870A50896192}"/>
+    <hyperlink ref="B19" r:id="rId16" xr:uid="{BFB067BC-CB15-45F3-8D98-A2808E40A2D1}"/>
+    <hyperlink ref="B20" r:id="rId17" xr:uid="{B84A9B9D-4CA1-4D31-ABD2-270DB3E159A5}"/>
+    <hyperlink ref="B21" r:id="rId18" xr:uid="{CD1C4BDA-81EC-49BB-955F-2655D9F6093D}"/>
+    <hyperlink ref="B22" r:id="rId19" xr:uid="{A9A64C56-EB2C-4EF7-97E8-E0DB6B10F6A9}"/>
+    <hyperlink ref="B23" r:id="rId20" xr:uid="{5505081D-A12C-4865-9A0D-92A65DACC264}"/>
+    <hyperlink ref="B24" r:id="rId21" xr:uid="{8F00F67C-9AE4-4EDF-9355-1D36F703CD54}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2907,19 +4158,19 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="C2" sqref="C2:C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.68359375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="82.89453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="53.26171875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.3671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="88.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="57" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.453125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2936,7 +4187,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>45</v>
       </c>
@@ -2945,18 +4196,18 @@
       <c r="D2" s="2"/>
       <c r="E2" s="6"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="7"/>
       <c r="B3" s="14" t="s">
-        <v>119</v>
+        <v>104</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>120</v>
+        <v>105</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="4"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>47</v>
       </c>
@@ -2965,41 +4216,41 @@
       <c r="D4" s="2"/>
       <c r="E4" s="6"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="8" t="s">
         <v>48</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>171</v>
+        <v>147</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>121</v>
+        <v>106</v>
       </c>
       <c r="D5" s="7"/>
       <c r="E5" s="4"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B6" s="14" t="s">
-        <v>172</v>
+        <v>148</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B7" s="14" t="s">
-        <v>173</v>
+        <v>149</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B8" s="14" t="s">
-        <v>174</v>
+        <v>150</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>124</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -3018,18 +4269,18 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="C2" sqref="C2:C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="66.05078125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="49.05078125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.3671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="66.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="52.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.453125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3046,7 +4297,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>45</v>
       </c>
@@ -3055,18 +4306,18 @@
       <c r="D2" s="2"/>
       <c r="E2" s="6"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="7"/>
       <c r="B3" s="7" t="s">
-        <v>118</v>
+        <v>103</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>115</v>
+        <v>100</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="4"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>47</v>
       </c>
@@ -3075,30 +4326,30 @@
       <c r="D4" s="2"/>
       <c r="E4" s="6"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="8" t="s">
         <v>48</v>
       </c>
       <c r="B5" t="s">
-        <v>158</v>
+        <v>134</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>117</v>
+        <v>102</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>116</v>
+        <v>101</v>
       </c>
       <c r="E5" s="4"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
-        <v>157</v>
+        <v>133</v>
       </c>
       <c r="C6" t="s">
-        <v>159</v>
+        <v>135</v>
       </c>
       <c r="D6" t="s">
-        <v>160</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>
@@ -3112,108 +4363,121 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A34C4D0B-5AF3-46AB-968C-E3C2E4AE293A}">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="66.05078125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="45.89453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.3671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.7265625" style="4"/>
+    <col min="2" max="2" width="69.81640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.453125" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.453125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="53.26953125" style="4" customWidth="1"/>
+    <col min="6" max="16384" width="8.7265625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="21" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="6"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B2" s="24"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="24"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="7"/>
       <c r="B3" s="7" t="s">
-        <v>112</v>
+        <v>97</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>113</v>
+        <v>98</v>
       </c>
       <c r="D3" s="7"/>
-      <c r="E3" s="4"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="3" t="s">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="B4" s="6"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="6"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B4" s="24"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="24"/>
+    </row>
+    <row r="5" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A5" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="B5" s="14" t="s">
-        <v>161</v>
+      <c r="B5" s="26" t="s">
+        <v>137</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>114</v>
+        <v>99</v>
       </c>
       <c r="D5" s="7"/>
-      <c r="E5" s="4"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="B6" s="14" t="s">
-        <v>162</v>
-      </c>
-      <c r="C6" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="B7" s="14" t="s">
-        <v>166</v>
-      </c>
-      <c r="C7" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="B8" s="14" t="s">
-        <v>167</v>
-      </c>
-      <c r="C8" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="C13" s="14"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="B14" s="14"/>
+      <c r="E5" s="19" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+      <c r="B6" s="26" t="s">
+        <v>138</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="E6" s="17" t="s">
+        <v>221</v>
+      </c>
+      <c r="F6" s="17"/>
+    </row>
+    <row r="7" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="B7" s="26" t="s">
+        <v>142</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="E7" s="17" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+      <c r="B8" s="26" t="s">
+        <v>143</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="E8" s="17" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C13" s="26"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B14" s="26"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -3232,18 +4496,18 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="C2" sqref="C2:C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="60.89453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="45.89453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.3671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="65.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.453125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3260,7 +4524,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>45</v>
       </c>
@@ -3269,18 +4533,18 @@
       <c r="D2" s="2"/>
       <c r="E2" s="6"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="7"/>
       <c r="B3" s="7" t="s">
-        <v>109</v>
+        <v>94</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>110</v>
+        <v>95</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="4"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>47</v>
       </c>
@@ -3289,40 +4553,57 @@
       <c r="D4" s="2"/>
       <c r="E4" s="6"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="8" t="s">
         <v>48</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="C5" s="7"/>
+        <v>96</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>315</v>
+      </c>
       <c r="D5" s="7"/>
       <c r="E5" s="4"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B6" s="7" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+        <v>292</v>
+      </c>
+      <c r="C6" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+        <v>151</v>
+      </c>
+      <c r="C7" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+        <v>152</v>
+      </c>
+      <c r="C8" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+        <v>153</v>
+      </c>
+      <c r="C9" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
-        <v>179</v>
+        <v>154</v>
+      </c>
+      <c r="C10" t="s">
+        <v>318</v>
       </c>
     </row>
   </sheetData>
@@ -3334,10 +4615,25 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101005D13AC7DC9987249A9E100E57525BE0A" ma:contentTypeVersion="6" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="33cc4cf79457d6899e34715919857312">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="5b8b0dab-f992-4a6f-a99a-885ec762b503" xmlns:ns3="90fead69-4c3a-4d4e-b099-377171a192c4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8f3c937d654d32362bc5f3f024806cc0" ns2:_="" ns3:_="">
-    <xsd:import namespace="5b8b0dab-f992-4a6f-a99a-885ec762b503"/>
-    <xsd:import namespace="90fead69-4c3a-4d4e-b099-377171a192c4"/>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x01010056A3F293FF3A9A4B98E64BB34BB78BA3" ma:contentTypeVersion="10" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="6f7d884989618a8400ceae295aa2c3bf">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="0c869d80-d99c-4dac-b26b-cbbc56b0e91c" xmlns:ns3="4a230dd3-5426-44e9-972e-c86e457e3d31" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="fd893c905c3e2cf3ffbdda313295f6b9" ns2:_="" ns3:_="">
+    <xsd:import namespace="0c869d80-d99c-4dac-b26b-cbbc56b0e91c"/>
+    <xsd:import namespace="4a230dd3-5426-44e9-972e-c86e457e3d31"/>
     <xsd:element name="properties">
       <xsd:complexType>
         <xsd:sequence>
@@ -3348,8 +4644,12 @@
                 <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceAutoTags" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceLocation" minOccurs="0"/>
                 <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
                 <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -3357,7 +4657,7 @@
       </xsd:complexType>
     </xsd:element>
   </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="5b8b0dab-f992-4a6f-a99a-885ec762b503" elementFormDefault="qualified">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="0c869d80-d99c-4dac-b26b-cbbc56b0e91c" elementFormDefault="qualified">
     <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
@@ -3370,23 +4670,43 @@
         <xsd:restriction base="dms:Note"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaServiceAutoTags" ma:index="10" nillable="true" ma:displayName="Tags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
+    <xsd:element name="MediaServiceAutoTags" ma:index="10" nillable="true" ma:displayName="MediaServiceAutoTags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaServiceOCR" ma:index="11" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+    <xsd:element name="MediaServiceOCR" ma:index="11" nillable="true" ma:displayName="MediaServiceOCR" ma:internalName="MediaServiceOCR" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note">
           <xsd:maxLength value="255"/>
         </xsd:restriction>
       </xsd:simpleType>
     </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="12" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceLocation" ma:index="13" nillable="true" ma:displayName="MediaServiceLocation" ma:internalName="MediaServiceLocation" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="16" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="17" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
   </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="90fead69-4c3a-4d4e-b099-377171a192c4" elementFormDefault="qualified">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="4a230dd3-5426-44e9-972e-c86e457e3d31" elementFormDefault="qualified">
     <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="SharedWithUsers" ma:index="12" nillable="true" ma:displayName="Compartido con" ma:internalName="SharedWithUsers" ma:readOnly="true">
+    <xsd:element name="SharedWithUsers" ma:index="14" nillable="true" ma:displayName="Compartido con" ma:internalName="SharedWithUsers" ma:readOnly="true">
       <xsd:complexType>
         <xsd:complexContent>
           <xsd:extension base="dms:UserMulti">
@@ -3405,7 +4725,7 @@
         </xsd:complexContent>
       </xsd:complexType>
     </xsd:element>
-    <xsd:element name="SharedWithDetails" ma:index="13" nillable="true" ma:displayName="Detalles de uso compartido" ma:internalName="SharedWithDetails" ma:readOnly="true">
+    <xsd:element name="SharedWithDetails" ma:index="15" nillable="true" ma:displayName="Detalles de uso compartido" ma:internalName="SharedWithDetails" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note">
           <xsd:maxLength value="255"/>
@@ -3512,30 +4832,40 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E2C7F53A-8E89-4CCC-9F6C-1071910C1BD9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="0c869d80-d99c-4dac-b26b-cbbc56b0e91c"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="4a230dd3-5426-44e9-972e-c86e457e3d31"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{67DC0167-6166-49C1-807E-C2398B5CAF50}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{087B298B-D9F4-4238-AB54-1DD9A78B2496}">
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B672E8A2-39C0-4B38-B673-715E4D9E7A1E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
     <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="5b8b0dab-f992-4a6f-a99a-885ec762b503"/>
-    <ds:schemaRef ds:uri="90fead69-4c3a-4d4e-b099-377171a192c4"/>
+    <ds:schemaRef ds:uri="0c869d80-d99c-4dac-b26b-cbbc56b0e91c"/>
+    <ds:schemaRef ds:uri="4a230dd3-5426-44e9-972e-c86e457e3d31"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
@@ -3544,29 +4874,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E2C7F53A-8E89-4CCC-9F6C-1071910C1BD9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="5b8b0dab-f992-4a6f-a99a-885ec762b503"/>
-    <ds:schemaRef ds:uri="90fead69-4c3a-4d4e-b099-377171a192c4"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{67DC0167-6166-49C1-807E-C2398B5CAF50}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>